<commit_message>
remap the order of conn
</commit_message>
<xml_diff>
--- a/5bus_Saadat.xlsx
+++ b/5bus_Saadat.xlsx
@@ -1603,8 +1603,8 @@
   </sheetPr>
   <dimension ref="A1:AH4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB2" activeCellId="0" sqref="AB2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1723,10 +1723,10 @@
         <v>52</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>11</v>
+        <v>135</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>11</v>
+        <v>135</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>100</v>
@@ -1806,10 +1806,10 @@
         <v>52</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>11</v>
+        <v>135</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>11</v>
+        <v>135</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>100</v>
@@ -1888,7 +1888,7 @@
   </sheetPr>
   <dimension ref="A1:Y42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="U3" activeCellId="0" sqref="U3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
nice order conn, needed offset
</commit_message>
<xml_diff>
--- a/5bus_Saadat.xlsx
+++ b/5bus_Saadat.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="232">
   <si>
     <t xml:space="preserve">Property</t>
   </si>
@@ -1603,8 +1603,8 @@
   </sheetPr>
   <dimension ref="A1:AH4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AB3" activeCellId="0" sqref="AB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1888,8 +1888,8 @@
   </sheetPr>
   <dimension ref="A1:Y42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U3" activeCellId="0" sqref="U3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X3" activeCellId="0" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1966,7 +1966,9 @@
       <c r="W1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="X1" s="1"/>
+      <c r="X1" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="Y1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2036,6 +2038,9 @@
       <c r="W2" s="0" t="s">
         <v>173</v>
       </c>
+      <c r="X2" s="0" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -2104,6 +2109,9 @@
       <c r="W3" s="0" t="s">
         <v>173</v>
       </c>
+      <c r="X3" s="0" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -2171,6 +2179,9 @@
       </c>
       <c r="W4" s="0" t="s">
         <v>173</v>
+      </c>
+      <c r="X4" s="0" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>